<commit_message>
Corrección de spreadsheet para ejecutar el mapping
</commit_message>
<xml_diff>
--- a/vocabulary/InputPhotocalysisMapping.xlsx
+++ b/vocabulary/InputPhotocalysisMapping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Prefix" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -68,6 +68,12 @@
     <t xml:space="preserve">http://purl.org/dc/terms/</t>
   </si>
   <si>
+    <t xml:space="preserve">schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://schema.org/</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID</t>
   </si>
   <si>
@@ -83,6 +89,15 @@
     <t xml:space="preserve">http://data.example.com/journal/{ID}</t>
   </si>
   <si>
+    <t xml:space="preserve">Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:Article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://doi.org/{DOI}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature</t>
   </si>
   <si>
@@ -93,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">journals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">paper_references</t>
   </si>
   <si>
     <t xml:space="preserve">Predicate</t>
@@ -119,6 +137,54 @@
     <t xml:space="preserve">{name}</t>
   </si>
   <si>
+    <t xml:space="preserve">string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:doi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{DOI}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{title}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:abstract</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Abstract}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:volume</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Volume}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">positiveInteger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:issue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Issue}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dcterms:date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Year}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bibo:pageStart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{Pages}</t>
+  </si>
+  <si>
     <t xml:space="preserve">FunctionID</t>
   </si>
 </sst>
@@ -129,7 +195,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -161,18 +227,32 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <u val="single"/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF1155CC"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <name val="calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
@@ -226,7 +306,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -243,7 +323,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -251,11 +351,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -336,13 +436,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z8"/>
+  <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A4:C8 B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="82.67"/>
@@ -430,9 +530,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+    </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1431,6 +1544,7 @@
     <hyperlink ref="B5" r:id="rId4" display="http://base.namespace.com/"/>
     <hyperlink ref="B6" r:id="rId5" display="http://purl.org/ontology/bibo/"/>
     <hyperlink ref="B7" r:id="rId6" display="http://purl.org/dc/terms/"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://schema.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1447,42 +1561,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="26.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="3" style="0" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2496,42 +2623,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="A4:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="10.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="16.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="10.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="8" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
+      <c r="A1" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>22</v>
+      <c r="B3" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3545,108 +3685,205 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="A4:C8 D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="26.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="0" width="8.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="33.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="37.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="16.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="8" width="25.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="8" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="8" width="19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="8" width="26.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="8" style="8" width="8.78"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="27" style="8" width="11.23"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
+      <c r="A2" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B3" s="6"/>
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B4" s="6"/>
+      <c r="A4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6"/>
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="6"/>
-      <c r="G6" s="6"/>
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="6"/>
-      <c r="G7" s="6"/>
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="6"/>
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6"/>
+      <c r="A9" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6"/>
+      <c r="B10" s="11"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6"/>
+      <c r="B11" s="11"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6"/>
+      <c r="B12" s="11"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="6"/>
+      <c r="B13" s="11"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="6"/>
+      <c r="B14" s="11"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6"/>
+      <c r="B15" s="11"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D24" s="0"/>
+    </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4639,13 +4876,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:C8 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.67"/>
@@ -4655,14 +4892,14 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>20</v>
+      <c r="A1" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Añadias primeras interacciones al mapping
- mappeo de journals
- comienzo de artículos
- relación con vista de autores
- sujetos del resto de elementos
</commit_message>
<xml_diff>
--- a/vocabulary/InputPhotocalysisMapping.xlsx
+++ b/vocabulary/InputPhotocalysisMapping.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="64">
   <si>
     <t xml:space="preserve">Prefix</t>
   </si>
@@ -98,6 +98,24 @@
     <t xml:space="preserve">https://doi.org/{DOI}</t>
   </si>
   <si>
+    <t xml:space="preserve">Author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/author/{author_name}-{ID}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MaterialTransformationProcess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">phcat:MaterialTransformationProcess</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://data.example.com/materialTransformastionProcess/{No_de_ref}</t>
+  </si>
+  <si>
     <t xml:space="preserve">Feature</t>
   </si>
   <si>
@@ -113,6 +131,12 @@
     <t xml:space="preserve">paper_references</t>
   </si>
   <si>
+    <t xml:space="preserve">phcat_authors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalystsdata</t>
+  </si>
+  <si>
     <t xml:space="preserve">Predicate</t>
   </si>
   <si>
@@ -183,6 +207,12 @@
   </si>
   <si>
     <t xml:space="preserve">{Pages}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema:name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{author_name}</t>
   </si>
   <si>
     <t xml:space="preserve">FunctionID</t>
@@ -439,7 +469,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A4:C8 B19"/>
+      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="A6:C8 B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1564,14 +1594,14 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A4:C8"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="28.91"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="61.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="0" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="7" style="0" width="8.78"/>
   </cols>
@@ -1610,8 +1640,28 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2608,6 +2658,10 @@
     <row r="999" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" display="http://data.example.com/author/"/>
+    <hyperlink ref="C5" r:id="rId2" display="http://data.example.com/materialTransformastionProcess/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -2626,12 +2680,12 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="A4:C8"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="A6:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="23.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="28.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="10.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="8" width="16.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="4" style="8" width="10.44"/>
@@ -2644,10 +2698,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2655,10 +2709,10 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2666,14 +2720,34 @@
         <v>21</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3688,7 +3762,7 @@
   <dimension ref="A1:G1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="1" sqref="A4:C8 D26"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="1" sqref="A6:C8 D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3709,22 +3783,22 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3732,13 +3806,13 @@
         <v>18</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3746,13 +3820,13 @@
         <v>21</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3760,13 +3834,13 @@
         <v>21</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3774,13 +3848,13 @@
         <v>21</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3788,13 +3862,13 @@
         <v>21</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="G6" s="11"/>
     </row>
@@ -3803,13 +3877,13 @@
         <v>21</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="G7" s="11"/>
     </row>
@@ -3818,13 +3892,13 @@
         <v>21</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3832,17 +3906,25 @@
         <v>21</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="11"/>
+      <c r="A10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="11"/>
@@ -4879,7 +4961,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A4:C8 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A6:C8 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.29296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4893,13 +4975,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="C1" s="12" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>